<commit_message>
add replace negative data
</commit_message>
<xml_diff>
--- a/database/industries/palayesh/shavan/product/monthly.xlsx
+++ b/database/industries/palayesh/shavan/product/monthly.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="c:\Users\EBRAHIMI\Desktop\Trade\database\industries\palayesh\shavan\product\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Trade\database\industries\palayesh\shavan\product\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C372E673-C673-45B5-A98F-34E90D3A11DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11025" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11025"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2662" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2662" uniqueCount="92">
   <si>
     <t>Pouya Finance</t>
   </si>
@@ -211,9 +210,6 @@
     <t>گاز مایع</t>
   </si>
   <si>
-    <t>بنزین معمولی</t>
-  </si>
-  <si>
     <t>نفتای سنگین</t>
   </si>
   <si>
@@ -235,9 +231,6 @@
     <t>هیدرو کربن MC160</t>
   </si>
   <si>
-    <t>بنزین یورو 5</t>
-  </si>
-  <si>
     <t>گوگرد .</t>
   </si>
   <si>
@@ -245,9 +238,6 @@
   </si>
   <si>
     <t>نفتای سنگین ترش</t>
-  </si>
-  <si>
-    <t>بنزین معمولی و یورو 5</t>
   </si>
   <si>
     <t>نفتای کامل</t>
@@ -303,11 +293,14 @@
   <si>
     <t>تن / ریال</t>
   </si>
+  <si>
+    <t>بنزین</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -779,10 +772,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:BB119"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2248,7 +2243,7 @@
     </row>
     <row r="16" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B16" s="12" t="s">
-        <v>63</v>
+        <v>91</v>
       </c>
       <c r="C16" s="13" t="s">
         <v>56</v>
@@ -2407,7 +2402,7 @@
     </row>
     <row r="17" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B17" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C17" s="11" t="s">
         <v>56</v>
@@ -2566,7 +2561,7 @@
     </row>
     <row r="18" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B18" s="12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C18" s="13" t="s">
         <v>56</v>
@@ -2725,7 +2720,7 @@
     </row>
     <row r="19" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B19" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C19" s="11" t="s">
         <v>56</v>
@@ -2884,7 +2879,7 @@
     </row>
     <row r="20" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B20" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C20" s="13" t="s">
         <v>56</v>
@@ -3043,7 +3038,7 @@
     </row>
     <row r="21" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B21" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C21" s="11" t="s">
         <v>56</v>
@@ -3202,7 +3197,7 @@
     </row>
     <row r="22" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B22" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C22" s="13" t="s">
         <v>56</v>
@@ -3361,7 +3356,7 @@
     </row>
     <row r="23" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B23" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C23" s="11" t="s">
         <v>56</v>
@@ -3520,7 +3515,7 @@
     </row>
     <row r="24" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B24" s="12" t="s">
-        <v>71</v>
+        <v>91</v>
       </c>
       <c r="C24" s="13" t="s">
         <v>56</v>
@@ -3679,7 +3674,7 @@
     </row>
     <row r="25" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B25" s="10" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C25" s="11" t="s">
         <v>56</v>
@@ -3838,7 +3833,7 @@
     </row>
     <row r="26" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B26" s="12" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C26" s="13" t="s">
         <v>56</v>
@@ -3997,7 +3992,7 @@
     </row>
     <row r="27" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B27" s="10" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C27" s="11" t="s">
         <v>56</v>
@@ -4156,7 +4151,7 @@
     </row>
     <row r="28" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B28" s="12" t="s">
-        <v>75</v>
+        <v>91</v>
       </c>
       <c r="C28" s="13" t="s">
         <v>56</v>
@@ -4315,7 +4310,7 @@
     </row>
     <row r="29" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B29" s="10" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C29" s="11" t="s">
         <v>56</v>
@@ -4474,7 +4469,7 @@
     </row>
     <row r="30" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B30" s="12" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C30" s="13" t="s">
         <v>56</v>
@@ -4633,7 +4628,7 @@
     </row>
     <row r="31" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B31" s="14" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C31" s="15"/>
       <c r="D31" s="15"/>
@@ -4690,7 +4685,7 @@
     </row>
     <row r="32" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B32" s="16" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C32" s="17"/>
       <c r="D32" s="17"/>
@@ -4847,7 +4842,7 @@
     </row>
     <row r="33" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B33" s="18" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C33" s="19"/>
       <c r="D33" s="19"/>
@@ -5169,7 +5164,7 @@
     </row>
     <row r="37" spans="2:54" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B37" s="7" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
@@ -5381,7 +5376,7 @@
     </row>
     <row r="39" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B39" s="8" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C39" s="9"/>
       <c r="D39" s="9"/>
@@ -6233,7 +6228,7 @@
     </row>
     <row r="45" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B45" s="12" t="s">
-        <v>63</v>
+        <v>91</v>
       </c>
       <c r="C45" s="13" t="s">
         <v>56</v>
@@ -6392,7 +6387,7 @@
     </row>
     <row r="46" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B46" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C46" s="11" t="s">
         <v>56</v>
@@ -6551,7 +6546,7 @@
     </row>
     <row r="47" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B47" s="12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C47" s="13" t="s">
         <v>56</v>
@@ -6710,7 +6705,7 @@
     </row>
     <row r="48" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B48" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C48" s="11" t="s">
         <v>56</v>
@@ -6869,7 +6864,7 @@
     </row>
     <row r="49" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B49" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C49" s="13" t="s">
         <v>56</v>
@@ -7028,7 +7023,7 @@
     </row>
     <row r="50" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B50" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C50" s="11" t="s">
         <v>56</v>
@@ -7187,7 +7182,7 @@
     </row>
     <row r="51" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B51" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C51" s="13" t="s">
         <v>56</v>
@@ -7346,7 +7341,7 @@
     </row>
     <row r="52" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B52" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C52" s="11" t="s">
         <v>56</v>
@@ -7505,7 +7500,7 @@
     </row>
     <row r="53" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B53" s="12" t="s">
-        <v>71</v>
+        <v>91</v>
       </c>
       <c r="C53" s="13" t="s">
         <v>56</v>
@@ -7664,7 +7659,7 @@
     </row>
     <row r="54" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B54" s="10" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C54" s="11" t="s">
         <v>56</v>
@@ -7823,7 +7818,7 @@
     </row>
     <row r="55" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B55" s="12" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C55" s="13" t="s">
         <v>56</v>
@@ -7982,7 +7977,7 @@
     </row>
     <row r="56" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B56" s="10" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C56" s="11" t="s">
         <v>56</v>
@@ -8141,7 +8136,7 @@
     </row>
     <row r="57" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B57" s="12" t="s">
-        <v>75</v>
+        <v>91</v>
       </c>
       <c r="C57" s="13" t="s">
         <v>56</v>
@@ -8300,7 +8295,7 @@
     </row>
     <row r="58" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B58" s="10" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C58" s="11" t="s">
         <v>56</v>
@@ -8459,7 +8454,7 @@
     </row>
     <row r="59" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B59" s="12" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C59" s="13" t="s">
         <v>56</v>
@@ -8618,7 +8613,7 @@
     </row>
     <row r="60" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B60" s="14" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C60" s="15"/>
       <c r="D60" s="15"/>
@@ -8675,7 +8670,7 @@
     </row>
     <row r="61" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B61" s="16" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C61" s="17"/>
       <c r="D61" s="17"/>
@@ -8832,7 +8827,7 @@
     </row>
     <row r="62" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B62" s="14" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C62" s="15"/>
       <c r="D62" s="15"/>
@@ -8889,7 +8884,7 @@
     </row>
     <row r="63" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B63" s="16" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C63" s="17"/>
       <c r="D63" s="17"/>
@@ -9046,7 +9041,7 @@
     </row>
     <row r="64" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B64" s="18" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C64" s="19"/>
       <c r="D64" s="19"/>
@@ -9368,7 +9363,7 @@
     </row>
     <row r="68" spans="2:54" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B68" s="7" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C68" s="6"/>
       <c r="D68" s="6"/>
@@ -9580,7 +9575,7 @@
     </row>
     <row r="70" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B70" s="8" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C70" s="9"/>
       <c r="D70" s="9"/>
@@ -9640,7 +9635,7 @@
         <v>55</v>
       </c>
       <c r="C71" s="11" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D71" s="11"/>
       <c r="E71" s="11" t="s">
@@ -9799,7 +9794,7 @@
         <v>58</v>
       </c>
       <c r="C72" s="13" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D72" s="13"/>
       <c r="E72" s="13">
@@ -9958,7 +9953,7 @@
         <v>59</v>
       </c>
       <c r="C73" s="11" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D73" s="11"/>
       <c r="E73" s="11">
@@ -10117,7 +10112,7 @@
         <v>61</v>
       </c>
       <c r="C74" s="13" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D74" s="13"/>
       <c r="E74" s="13" t="s">
@@ -10276,7 +10271,7 @@
         <v>62</v>
       </c>
       <c r="C75" s="11" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D75" s="11"/>
       <c r="E75" s="11">
@@ -10432,10 +10427,10 @@
     </row>
     <row r="76" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B76" s="12" t="s">
-        <v>63</v>
+        <v>91</v>
       </c>
       <c r="C76" s="13" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D76" s="13"/>
       <c r="E76" s="13">
@@ -10591,10 +10586,10 @@
     </row>
     <row r="77" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B77" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C77" s="11" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D77" s="11"/>
       <c r="E77" s="11" t="s">
@@ -10750,10 +10745,10 @@
     </row>
     <row r="78" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B78" s="12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C78" s="13" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D78" s="13"/>
       <c r="E78" s="13" t="s">
@@ -10909,10 +10904,10 @@
     </row>
     <row r="79" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B79" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C79" s="11" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D79" s="11"/>
       <c r="E79" s="11">
@@ -11068,10 +11063,10 @@
     </row>
     <row r="80" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B80" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C80" s="13" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D80" s="13"/>
       <c r="E80" s="13">
@@ -11227,10 +11222,10 @@
     </row>
     <row r="81" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B81" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C81" s="11" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D81" s="11"/>
       <c r="E81" s="11">
@@ -11386,10 +11381,10 @@
     </row>
     <row r="82" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B82" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C82" s="13" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D82" s="13"/>
       <c r="E82" s="13">
@@ -11545,10 +11540,10 @@
     </row>
     <row r="83" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B83" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C83" s="11" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D83" s="11"/>
       <c r="E83" s="11">
@@ -11704,10 +11699,10 @@
     </row>
     <row r="84" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B84" s="12" t="s">
-        <v>71</v>
+        <v>91</v>
       </c>
       <c r="C84" s="13" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D84" s="13"/>
       <c r="E84" s="13" t="s">
@@ -11863,10 +11858,10 @@
     </row>
     <row r="85" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B85" s="10" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C85" s="11" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D85" s="11"/>
       <c r="E85" s="11" t="s">
@@ -12022,10 +12017,10 @@
     </row>
     <row r="86" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B86" s="12" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C86" s="13" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D86" s="13"/>
       <c r="E86" s="13" t="s">
@@ -12181,10 +12176,10 @@
     </row>
     <row r="87" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B87" s="10" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C87" s="11" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D87" s="11"/>
       <c r="E87" s="11" t="s">
@@ -12340,10 +12335,10 @@
     </row>
     <row r="88" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B88" s="12" t="s">
-        <v>75</v>
+        <v>91</v>
       </c>
       <c r="C88" s="13" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D88" s="13"/>
       <c r="E88" s="13" t="s">
@@ -12499,10 +12494,10 @@
     </row>
     <row r="89" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B89" s="10" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C89" s="11" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D89" s="11"/>
       <c r="E89" s="11" t="s">
@@ -12658,10 +12653,10 @@
     </row>
     <row r="90" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B90" s="12" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C90" s="13" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D90" s="13"/>
       <c r="E90" s="13" t="s">
@@ -12817,7 +12812,7 @@
     </row>
     <row r="91" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B91" s="14" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C91" s="15"/>
       <c r="D91" s="15"/>
@@ -12874,10 +12869,10 @@
     </row>
     <row r="92" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B92" s="16" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C92" s="17" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D92" s="17"/>
       <c r="E92" s="17" t="s">
@@ -13033,7 +13028,7 @@
     </row>
     <row r="93" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B93" s="14" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C93" s="15"/>
       <c r="D93" s="15"/>
@@ -13090,10 +13085,10 @@
     </row>
     <row r="94" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B94" s="16" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C94" s="17" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D94" s="17"/>
       <c r="E94" s="17" t="s">
@@ -13249,7 +13244,7 @@
     </row>
     <row r="95" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B95" s="8" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C95" s="9"/>
       <c r="D95" s="9"/>
@@ -13306,10 +13301,10 @@
     </row>
     <row r="96" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B96" s="10" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C96" s="11" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D96" s="11"/>
       <c r="E96" s="11" t="s">
@@ -13465,7 +13460,7 @@
     </row>
     <row r="97" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B97" s="18" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C97" s="19"/>
       <c r="D97" s="19"/>
@@ -13787,7 +13782,7 @@
     </row>
     <row r="101" spans="2:54" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B101" s="7" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C101" s="6"/>
       <c r="D101" s="6"/>
@@ -13999,7 +13994,7 @@
     </row>
     <row r="103" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B103" s="8" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C103" s="9"/>
       <c r="D103" s="9"/>
@@ -14059,7 +14054,7 @@
         <v>58</v>
       </c>
       <c r="C104" s="11" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D104" s="11"/>
       <c r="E104" s="11">
@@ -14218,7 +14213,7 @@
         <v>59</v>
       </c>
       <c r="C105" s="13" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D105" s="13"/>
       <c r="E105" s="13">
@@ -14377,7 +14372,7 @@
         <v>61</v>
       </c>
       <c r="C106" s="11" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D106" s="11"/>
       <c r="E106" s="11" t="s">
@@ -14536,7 +14531,7 @@
         <v>62</v>
       </c>
       <c r="C107" s="13" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D107" s="13"/>
       <c r="E107" s="13">
@@ -14692,10 +14687,10 @@
     </row>
     <row r="108" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B108" s="10" t="s">
-        <v>63</v>
+        <v>91</v>
       </c>
       <c r="C108" s="11" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D108" s="11"/>
       <c r="E108" s="11">
@@ -14851,10 +14846,10 @@
     </row>
     <row r="109" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B109" s="12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C109" s="13" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D109" s="13"/>
       <c r="E109" s="13" t="s">
@@ -15010,10 +15005,10 @@
     </row>
     <row r="110" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B110" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C110" s="11" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D110" s="11"/>
       <c r="E110" s="11">
@@ -15169,10 +15164,10 @@
     </row>
     <row r="111" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B111" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C111" s="13" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D111" s="13"/>
       <c r="E111" s="13">
@@ -15328,10 +15323,10 @@
     </row>
     <row r="112" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B112" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C112" s="11" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D112" s="11"/>
       <c r="E112" s="11">
@@ -15487,10 +15482,10 @@
     </row>
     <row r="113" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B113" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C113" s="13" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D113" s="13"/>
       <c r="E113" s="13">
@@ -15646,10 +15641,10 @@
     </row>
     <row r="114" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B114" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C114" s="11" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D114" s="11"/>
       <c r="E114" s="11">
@@ -15805,10 +15800,10 @@
     </row>
     <row r="115" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B115" s="12" t="s">
-        <v>71</v>
+        <v>91</v>
       </c>
       <c r="C115" s="13" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D115" s="13"/>
       <c r="E115" s="13" t="s">
@@ -15964,10 +15959,10 @@
     </row>
     <row r="116" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B116" s="10" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C116" s="11" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D116" s="11"/>
       <c r="E116" s="11" t="s">
@@ -16123,10 +16118,10 @@
     </row>
     <row r="117" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B117" s="12" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C117" s="13" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D117" s="13"/>
       <c r="E117" s="13" t="s">
@@ -16282,10 +16277,10 @@
     </row>
     <row r="118" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B118" s="10" t="s">
-        <v>75</v>
+        <v>91</v>
       </c>
       <c r="C118" s="11" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D118" s="11"/>
       <c r="E118" s="11" t="s">
@@ -16441,10 +16436,10 @@
     </row>
     <row r="119" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B119" s="12" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C119" s="13" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D119" s="13"/>
       <c r="E119" s="13" t="s">

</xml_diff>